<commit_message>
🔄 Actualización automática del index.html y archivo Excel
</commit_message>
<xml_diff>
--- a/mapa_interactivo_AYKO.xlsx
+++ b/mapa_interactivo_AYKO.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,27 +508,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2779</t>
+          <t>4915</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>GUEVARA 687</t>
+          <t>BARCA CABO DE HORNOS 6753</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>792041586</t>
+          <t>803607875</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -543,7 +543,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Falta traspaso y retiro</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -563,40 +563,40 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.453307</v>
+        <v>-58.491041</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.585706</v>
+        <v>-34.679704</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>5110</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>3/25/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MCAL SOLANO LOPEZ 3110</t>
+          <t>CUENCA 158</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>792101640</t>
+          <t>804287943</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Retirar columna. TLC ya traspaso nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -635,36 +635,36 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.498448</v>
+        <v>-58.474432</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.595287</v>
+        <v>-34.629827</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3269</t>
+          <t>5138</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9/9/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ANDALGALA 2590</t>
+          <t>LOPEZ, CARLOS ANTONIO 3326</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>796141865</t>
+          <t>804468459</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -679,7 +679,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Columna sobre plazoleta frente a altura 2590 - Ver foto para ubicar</t>
+          <t>COLUMNA INCLINADA</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -703,26 +703,26 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.502411</v>
+        <v>-58.508582</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.665815</v>
+        <v>-34.588936</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3765</t>
+          <t>5139</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>4/1/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NAZCA AV. 1675</t>
+          <t>LOPEZ, CARLOS ANTONIO 3346</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -732,7 +732,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>798295165</t>
+          <t>804468467</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Columna con base picada</t>
+          <t>COLUMNA INCLINADA</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -757,12 +757,12 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -771,36 +771,36 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.47874</v>
+        <v>-58.508809</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.61462</v>
+        <v>-34.589076</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>4399</t>
+          <t>5479</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>12/12/2024</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>AVALOS 1487</t>
+          <t>CONCORDIA 812</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>801644860</t>
+          <t>804497942</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -835,40 +835,40 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.478352</v>
+        <v>-58.479563</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.58305</v>
+        <v>-34.623886</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4423</t>
+          <t>5485</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>12/18/2024</t>
+          <t>4/4/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>VERA 1081</t>
+          <t>FLORES, VENANCIO, GRAL. 2977</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>801734625</t>
+          <t>804497954</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>PICADA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -903,40 +903,40 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.44244</v>
+        <v>-58.471643</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.593883</v>
+        <v>-34.629262</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4895</t>
+          <t>5500</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2/12/2025</t>
+          <t>4/7/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 1335</t>
+          <t>LA PLATA AV. 1013</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>803607583</t>
+          <t>804568914</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Quedo fuera de plomo</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -975,36 +975,36 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.460926</v>
+        <v>-58.426804</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.578223</v>
+        <v>-34.627283</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4915</t>
+          <t>3289</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>4/7/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BARCA CABO DE HORNOS 6753</t>
+          <t>TRES ARROYOS 251</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>803607875</t>
+          <t>804568949</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1039,40 +1039,40 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.491041</v>
+        <v>-58.447225</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.679704</v>
+        <v>-34.601357</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5110</t>
+          <t>5728</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3/25/2025</t>
+          <t>4/7/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CUENCA 158</t>
+          <t>FRANCO 3340</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>804287943</t>
+          <t>804568964</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1111,36 +1111,36 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.474432</v>
+        <v>-58.512525</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.629827</v>
+        <v>-34.585228</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>5521</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>EL PEREGRINO 3115</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>804569000</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Aplomar Poste</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1175,40 +1175,40 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.426593</v>
+        <v>-58.485232</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.628211</v>
+        <v>-34.611573</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>5572</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>SANABRIA 4289</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804663652</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1243,40 +1243,40 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.484185</v>
+        <v>-58.516755</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.582206</v>
+        <v>-34.6002</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3082</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CAMACUA 141</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>804309680</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1315,36 +1315,36 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.458015</v>
+        <v>-58.525125</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.629277</v>
+        <v>-34.604668</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>5574</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>GRIVEO 3909</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804663683</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste Inclinado</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1379,40 +1379,40 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.48396</v>
+        <v>-58.517126</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.582874</v>
+        <v>-34.592774</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5127</t>
+          <t>5642</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LAMARCA, EMILIO 224</t>
+          <t>ALVAREZ THOMAS AV. 1212</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>804323949</t>
+          <t>804876050</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1451,26 +1451,26 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.477988</v>
+        <v>-58.458816</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.630001</v>
+        <v>-34.578469</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>5664</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>BOGOTA 2936</t>
+          <t>REMEDIOS 2675</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>804323945</t>
+          <t>805507228</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1519,36 +1519,36 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.4716</v>
+        <v>-58.463339</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.627623</v>
+        <v>-34.6369</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5138</t>
+          <t>5668</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LOPEZ, CARLOS ANTONIO 3326</t>
+          <t>CURAPALIGUE 367</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>804468459</t>
+          <t>805507231</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>COLUMNA INCLINADA</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1587,26 +1587,26 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.508582</v>
+        <v>-58.452319</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.588936</v>
+        <v>-34.62917</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5139</t>
+          <t>5805</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/1/2025</t>
+          <t>5/14/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>LOPEZ, CARLOS ANTONIO 3346</t>
+          <t>GUTENBERG 4134</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804468467</t>
+          <t>806926378</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>COLUMNA INCLINADA</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1651,40 +1651,40 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.508809</v>
+        <v>-58.51665</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.589076</v>
+        <v>-34.596644</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5479</t>
+          <t>5828</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/4/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CONCORDIA 812</t>
+          <t>VERA 121</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804497942</t>
+          <t>806926459</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1723,961 +1723,9 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.479563</v>
+        <v>-58.434686</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.623886</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>5485</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>4/4/2025</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>FLORES, VENANCIO, GRAL. 2977</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>804497954</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M20" t="n">
-        <v>-58.471643</v>
-      </c>
-      <c r="N20" t="n">
-        <v>-34.629262</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>5500</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>4/7/2025</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>LA PLATA AV. 1013</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>804568914</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Aplomar</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M21" t="n">
-        <v>-58.426804</v>
-      </c>
-      <c r="N21" t="n">
-        <v>-34.627283</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>3289</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>4/7/2025</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>TRES ARROYOS 251</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>804568949</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M22" t="n">
-        <v>-58.447225</v>
-      </c>
-      <c r="N22" t="n">
-        <v>-34.601357</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>5728</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>4/7/2025</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>FRANCO 3340</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>804568964</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M23" t="n">
-        <v>-58.512525</v>
-      </c>
-      <c r="N23" t="n">
-        <v>-34.585228</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>5521</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>4/8/2025</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>EL PEREGRINO 3115</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>804569000</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Aplomar Poste</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M24" t="n">
-        <v>-58.485232</v>
-      </c>
-      <c r="N24" t="n">
-        <v>-34.611573</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>5572</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>4/14/2025</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>SANABRIA 4289</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>804663652</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>Poste inclinado</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M25" t="n">
-        <v>-58.516755</v>
-      </c>
-      <c r="N25" t="n">
-        <v>-34.6002</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>5573</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>4/14/2025</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>LASTRA AV. 4379</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>804663677</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M26" t="n">
-        <v>-58.525125</v>
-      </c>
-      <c r="N26" t="n">
-        <v>-34.604668</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>5574</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>4/14/2025</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>GRIVEO 3909</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>804663683</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Poste Inclinado</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M27" t="n">
-        <v>-58.517126</v>
-      </c>
-      <c r="N27" t="n">
-        <v>-34.592774</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>5621</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>4/22/2025</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>MORON 4106</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>804876042</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Desplazar columna por entrada de vehiculos.</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M28" t="n">
-        <v>-58.487352</v>
-      </c>
-      <c r="N28" t="n">
-        <v>-34.627992</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>5642</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>4/22/2025</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>ALVAREZ THOMAS AV. 1212</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>804876050</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M29" t="n">
-        <v>-58.458816</v>
-      </c>
-      <c r="N29" t="n">
-        <v>-34.578469</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>5664</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>4/28/2025</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>REMEDIOS 2675</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>805507228</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M30" t="n">
-        <v>-58.463339</v>
-      </c>
-      <c r="N30" t="n">
-        <v>-34.6369</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>5668</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>4/28/2025</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>CURAPALIGUE 367</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>805507231</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M31" t="n">
-        <v>-58.452319</v>
-      </c>
-      <c r="N31" t="n">
-        <v>-34.62917</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>5805</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>5/14/2025</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>GUTENBERG 4134</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>806926378</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Poste inclinado</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
-      <c r="M32" t="n">
-        <v>-58.51665</v>
-      </c>
-      <c r="N32" t="n">
-        <v>-34.596644</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>5828</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>5/19/2025</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>VERA 121</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>806926459</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>AYKO</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M33" t="n">
-        <v>-58.434686</v>
-      </c>
-      <c r="N33" t="n">
         <v>-34.602057</v>
       </c>
     </row>

</xml_diff>